<commit_message>
use same applications in both test fixtures
</commit_message>
<xml_diff>
--- a/tests/fixtures/store/api/application_versions.xlsx
+++ b/tests/fixtures/store/api/application_versions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/store/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7831085E-FC59-1F44-AA58-009494246434}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED98C50C-0F0A-1847-9683-26DC6EF8F8BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="1160" windowWidth="27640" windowHeight="20780" xr2:uid="{FDA99A34-7115-4947-8987-A8BAD728483C}"/>
+    <workbookView xWindow="14380" yWindow="4520" windowWidth="27640" windowHeight="20780" xr2:uid="{FDA99A34-7115-4947-8987-A8BAD728483C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,19 +48,19 @@
     <t>Research</t>
   </si>
   <si>
-    <t>PGSPCFC030</t>
-  </si>
-  <si>
-    <t>PGSLIFC030</t>
-  </si>
-  <si>
-    <t>PGSPCFC060</t>
-  </si>
-  <si>
-    <t>PGSPCFC090</t>
-  </si>
-  <si>
-    <t>PGTPCFC030</t>
+    <t>PGOTTTR020</t>
+  </si>
+  <si>
+    <t>PGOTTTR030</t>
+  </si>
+  <si>
+    <t>PGOTTTR040</t>
+  </si>
+  <si>
+    <t>PGOTTTR060</t>
+  </si>
+  <si>
+    <t>PGOTTTR080</t>
   </si>
 </sst>
 </file>
@@ -71,7 +71,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _k_r_-;\-* #,##0.00\ _k_r_-;_-* &quot;-&quot;??\ _k_r_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -85,6 +85,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,10 +120,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,7 +444,7 @@
   <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,7 +477,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2">
@@ -486,7 +500,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B3">
@@ -509,7 +523,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4">
@@ -532,7 +546,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B5">
@@ -555,7 +569,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6">

</xml_diff>

<commit_message>
Feat(admin): making %kth requiered (#538)
* making %kth requiered

* fixing tests

* lint stuff

* black tests

* Code format with Black

* code format rest of changed files

Co-authored-by: Patrik Grenfeldt <patrik.grenfeldt@scilifelab.se>
</commit_message>
<xml_diff>
--- a/tests/fixtures/store/api/application_versions.xlsx
+++ b/tests/fixtures/store/api/application_versions.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/store/api/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED98C50C-0F0A-1847-9683-26DC6EF8F8BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28125"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14380" yWindow="4520" windowWidth="27640" windowHeight="20780" xr2:uid="{FDA99A34-7115-4947-8987-A8BAD728483C}"/>
+    <workbookView xWindow="14380" yWindow="4520" windowWidth="27640" windowHeight="20780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -25,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>App tag</t>
   </si>
@@ -61,17 +58,20 @@
   </si>
   <si>
     <t>PGOTTTR080</t>
+  </si>
+  <si>
+    <t>Percent kth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _k_r_-;\-* #,##0.00\ _k_r_-;_-* &quot;-&quot;??\ _k_r_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -98,6 +98,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -120,16 +133,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Tusental" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -187,7 +202,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -239,7 +254,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -433,27 +448,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{763E551C-82CE-874B-8FE0-5D57462FA358}">
-  <dimension ref="A1:G77"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,8 +490,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -498,8 +516,11 @@
       <c r="G2" s="2">
         <v>4700.3246648187996</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -521,8 +542,11 @@
       <c r="G3" s="2">
         <v>16329.924664818811</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -544,8 +568,11 @@
       <c r="G4" s="2">
         <v>24474.619897424811</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -567,8 +594,11 @@
       <c r="G5" s="2">
         <v>24435.581796697501</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -590,498 +620,501 @@
       <c r="G6" s="2">
         <v>2894.0280854306002</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:7">
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:7">
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:7">
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:7">
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:7">
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:7">
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:7">
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:7">
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:7">
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:7">
       <c r="C26" s="1"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:7">
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:7">
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:7">
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:7">
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:7">
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:7">
       <c r="C32" s="1"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:7">
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:7">
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:7">
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:7">
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:7">
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:7">
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:7">
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:7">
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:7">
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:7">
       <c r="C42" s="1"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:7">
       <c r="C43" s="1"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:7">
       <c r="C44" s="1"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:7">
       <c r="C45" s="1"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:7">
       <c r="C46" s="1"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:7">
       <c r="C47" s="1"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:7">
       <c r="C48" s="1"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:7">
       <c r="C49" s="1"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:7">
       <c r="C50" s="1"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:7">
       <c r="C51" s="1"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:7">
       <c r="C52" s="1"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:7">
       <c r="C53" s="1"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:7">
       <c r="C54" s="1"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:7">
       <c r="C55" s="1"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:7">
       <c r="C56" s="1"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:7">
       <c r="C57" s="1"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:7">
       <c r="C58" s="1"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:7">
       <c r="C59" s="1"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:7">
       <c r="C60" s="1"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:7">
       <c r="C61" s="1"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:7">
       <c r="C62" s="1"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:7">
       <c r="C63" s="1"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:7">
       <c r="C64" s="1"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:7">
       <c r="C65" s="1"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:7">
       <c r="C66" s="1"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:7">
       <c r="C67" s="1"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:7">
       <c r="C68" s="1"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:7">
       <c r="C69" s="1"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:7">
       <c r="C70" s="1"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:7">
       <c r="C71" s="1"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:7">
       <c r="C72" s="1"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:7">
       <c r="C73" s="1"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:7">
       <c r="C74" s="1"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:7">
       <c r="C75" s="1"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:7">
       <c r="C76" s="1"/>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:7">
       <c r="C77" s="1"/>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -1090,5 +1123,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>